<commit_message>
View in designer + fix template
</commit_message>
<xml_diff>
--- a/DataEntryFormSample/PayrollCalculatorTemplate.xlsx
+++ b/DataEntryFormSample/PayrollCalculatorTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DataEntryFormSample\DataEntryFormSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027A9D63-B0C8-46E0-9550-F1C7A7128C6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042E0184-D31E-4B04-8F58-DD2BF2C893D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CF7A" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73FB3FD1-26D8-4C14-9D27-733BB681B0DF}"/>
@@ -109,7 +109,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="#0_)"/>
+    <numFmt numFmtId="165" formatCode="#0_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -218,10 +218,6 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -231,8 +227,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -583,9 +583,9 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
-      <c r="J1" s="12" t="str">
+      <c r="J1" s="11" t="str">
         <f ca="1">CONCATENATE("Period: ",TEXT(NOW(), "M/d/yyyy"))</f>
-        <v>Period: 8/1/2019</v>
+        <v>Period: 8/2/2019</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -603,7 +603,7 @@
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1"/>
@@ -659,7 +659,7 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <v>40</v>
       </c>
       <c r="E8" s="3"/>
@@ -667,7 +667,7 @@
       <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>2.3E-2</v>
       </c>
       <c r="J8" s="3"/>
@@ -687,7 +687,7 @@
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="13">
         <v>5</v>
       </c>
       <c r="E10" s="3"/>
@@ -695,7 +695,7 @@
       <c r="H10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <v>0.28000000000000003</v>
       </c>
       <c r="J10" s="3"/>
@@ -715,7 +715,7 @@
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="13">
         <v>1</v>
       </c>
       <c r="E12" s="3"/>
@@ -723,7 +723,7 @@
       <c r="H12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>6.3E-2</v>
       </c>
       <c r="J12" s="3"/>
@@ -743,13 +743,15 @@
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <v>1.4500000000000001E-2</v>
       </c>
       <c r="J14" s="3"/>
@@ -769,13 +771,15 @@
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="15">
+        <v>0</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <f>SUM(I8,I10,I12,I14)</f>
         <v>0.38050000000000006</v>
       </c>
@@ -826,7 +830,7 @@
       <c r="H20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>20</v>
       </c>
       <c r="J20" s="3"/>
@@ -854,7 +858,7 @@
       <c r="H22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="8">
         <v>40</v>
       </c>
       <c r="J22" s="3"/>

</xml_diff>

<commit_message>
Sample data + binding
</commit_message>
<xml_diff>
--- a/DataEntryFormSample/PayrollCalculatorTemplate.xlsx
+++ b/DataEntryFormSample/PayrollCalculatorTemplate.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DataEntryFormSample\DataEntryFormSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042E0184-D31E-4B04-8F58-DD2BF2C893D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2B9EF3-1B61-4DEE-8310-43D9CBBC85F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CF7A" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73FB3FD1-26D8-4C14-9D27-733BB681B0DF}"/>
+    <workbookView xWindow="4110" yWindow="1575" windowWidth="17085" windowHeight="13245" xr2:uid="{73FB3FD1-26D8-4C14-9D27-733BB681B0DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Payroll Calculator" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#0_)"/>
+    <numFmt numFmtId="167" formatCode="&quot;Period: &quot;m\/d\/yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -221,9 +222,6 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -231,10 +229,13 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -583,10 +584,13 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
-      <c r="J1" s="11" t="str">
-        <f ca="1">CONCATENATE("Period: ",TEXT(NOW(), "M/d/yyyy"))</f>
-        <v>Period: 8/2/2019</v>
-      </c>
+      <c r="G1" s="15">
+        <f ca="1">NOW()</f>
+        <v>43682.406598148147</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
@@ -603,7 +607,7 @@
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1"/>
@@ -659,7 +663,7 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>40</v>
       </c>
       <c r="E8" s="3"/>
@@ -687,7 +691,7 @@
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <v>5</v>
       </c>
       <c r="E10" s="3"/>
@@ -715,7 +719,7 @@
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <v>1</v>
       </c>
       <c r="E12" s="3"/>
@@ -743,7 +747,7 @@
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <v>0</v>
       </c>
       <c r="E14" s="3"/>
@@ -771,7 +775,7 @@
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="13">
         <v>0</v>
       </c>
       <c r="E16" s="3"/>
@@ -905,8 +909,9 @@
     </row>
   </sheetData>
   <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>